<commit_message>
+Separate xamls for login,transaction and reading the data
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shireen.M\Documents\UiPath\REf_DataTable\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shireen.M\Documents\UiPath\Shireen_Day11_Assignment1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322F1CFA-46C9-4400-B84F-B9CB200257DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEFA347-B50A-42FF-B1DA-07DCEB61B55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -180,6 +180,30 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>OutputDataFilePath</t>
+  </si>
+  <si>
+    <t>Sheet2</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Exception</t>
+  </si>
+  <si>
+    <t>TransactionNumber</t>
+  </si>
+  <si>
+    <t>StatusColumn</t>
+  </si>
+  <si>
+    <t>ExceptionColumn</t>
+  </si>
+  <si>
+    <t>TransactionNumberColumn</t>
   </si>
 </sst>
 </file>
@@ -565,7 +589,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -660,10 +684,38 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
+Completed annotations as well as exception handling
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shireen.M\Documents\UiPath\Shireen_Day11_Assignment1\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\UiPath\Shireen_Day11_Assignment1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEFA347-B50A-42FF-B1DA-07DCEB61B55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AAEE11D-B7E0-4AB4-8AA0-7BA3D7E8C531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="72">
   <si>
     <t>Name</t>
   </si>
@@ -85,10 +85,6 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
@@ -113,9 +109,6 @@
     <t>OrchestratorAssetFolder</t>
   </si>
   <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
     <t>MaxConsecutiveSystemExceptions</t>
   </si>
   <si>
@@ -176,34 +169,76 @@
     <t>Data\Input\uidemo.exe</t>
   </si>
   <si>
-    <t>TransactionCell</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>OutputDataFilePath</t>
-  </si>
-  <si>
-    <t>Sheet2</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
     <t>Exception</t>
   </si>
   <si>
-    <t>TransactionNumber</t>
-  </si>
-  <si>
     <t>StatusColumn</t>
   </si>
   <si>
     <t>ExceptionColumn</t>
   </si>
   <si>
-    <t>TransactionNumberColumn</t>
+    <t>TimeOut</t>
+  </si>
+  <si>
+    <t>BusinessException</t>
+  </si>
+  <si>
+    <t>UserId and password doesnot match</t>
+  </si>
+  <si>
+    <t>SystemException</t>
+  </si>
+  <si>
+    <t>Application not loading</t>
+  </si>
+  <si>
+    <t>BusinessExceptionValues</t>
+  </si>
+  <si>
+    <t>The transaction values are not numeric</t>
+  </si>
+  <si>
+    <t>OutputDataSheet</t>
+  </si>
+  <si>
+    <t>Sheet3</t>
+  </si>
+  <si>
+    <t>Name of the file where the input excel is stored</t>
+  </si>
+  <si>
+    <t>Name of the input sheet</t>
+  </si>
+  <si>
+    <t>UiDemo application path</t>
+  </si>
+  <si>
+    <t>The sheet name in the input file where the output is stored</t>
+  </si>
+  <si>
+    <t>Name of the status column in the input file</t>
+  </si>
+  <si>
+    <t>Name of the exception column in the input file</t>
+  </si>
+  <si>
+    <t>Delay for the check App state activity</t>
+  </si>
+  <si>
+    <t>Message to be displayed when the business exception occurs in the login page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Message to be displayed when the system exception occurs </t>
+  </si>
+  <si>
+    <t>Message to be displayed when the business exception occurs in the transaction page</t>
+  </si>
+  <si>
+    <t>Asset where the userid and password is stored</t>
   </si>
 </sst>
 </file>
@@ -290,9 +325,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -330,7 +365,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -436,7 +471,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -578,7 +613,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -586,18 +621,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="63" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -636,88 +671,126 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="14.5">
       <c r="A3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="C6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>60</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>49</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" t="s">
-        <v>55</v>
+        <v>52</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" t="s">
         <v>56</v>
       </c>
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1701,8 +1774,6 @@
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1714,16 +1785,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1760,7 +1831,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1768,18 +1839,18 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1803,7 +1874,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1825,7 +1896,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1836,7 +1907,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1847,61 +1918,64 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2886,12 +2960,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" customWidth="1"/>
+    <col min="3" max="3" width="60.26953125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2902,7 +2976,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>